<commit_message>
Creación de ejecutable, agregar funciones de exportacion e importacion de archivos juntos con sus botones Version 3.
</commit_message>
<xml_diff>
--- a/data/datos.xlsx
+++ b/data/datos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,242 +492,107 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
+        <v>492</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>hoy</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>diana rodriguez</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>mañamna</t>
+        </is>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no se </t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>no se</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">medicina legal </t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>fractura</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B3" t="n">
-        <v>35</v>
-      </c>
-      <c r="C3" t="n">
-        <v>35</v>
-      </c>
-      <c r="D3" t="n">
-        <v>35</v>
-      </c>
-      <c r="E3" t="n">
-        <v>35</v>
-      </c>
-      <c r="F3" t="n">
-        <v>35</v>
-      </c>
-      <c r="G3" t="n">
-        <v>35</v>
-      </c>
-      <c r="H3" t="n">
-        <v>35</v>
-      </c>
-      <c r="I3" t="n">
-        <v>35</v>
-      </c>
-      <c r="J3" t="n">
-        <v>35</v>
-      </c>
-      <c r="K3" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2we</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>222</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>oido</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>3as</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>3asdasd</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>3</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>n</t>
         </is>
       </c>
     </row>

</xml_diff>